<commit_message>
Feature: Func to formate date
</commit_message>
<xml_diff>
--- a/RaceKey.xlsx
+++ b/RaceKey.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,498 +441,251 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>country_name</t>
+          <t>meeting_key</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>circuit_short_name</t>
+          <t>driver_number</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>date_start</t>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>position</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9472</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Bahrain</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Sakhir</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C2" t="n">
+        <v>63</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>02-03-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9480</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Saudi Arabia</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Jeddah</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C3" t="n">
+        <v>63</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>09-03-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9488</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Melbourne</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C4" t="n">
+        <v>63</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>24-03-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>9496</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Japan</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Suzuka</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C5" t="n">
+        <v>63</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>07-04-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9673</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>China</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Shanghai</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C6" t="n">
+        <v>63</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>21-04-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>9507</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Miami</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C7" t="n">
+        <v>63</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>05-05-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>9515</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Imola</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C8" t="n">
+        <v>63</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>19-05-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9523</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Monaco</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Monte Carlo</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C9" t="n">
+        <v>63</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>26-05-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9531</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Montreal</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C10" t="n">
+        <v>63</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>09-06-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9539</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Spain</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Catalunya</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C11" t="n">
+        <v>63</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>23-06-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>9550</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Austria</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Spielberg</t>
-        </is>
+      <c r="B12" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C12" t="n">
+        <v>63</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>30-06-2024</t>
         </is>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9558</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Great Britain</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Silverstone</t>
-        </is>
+        <v>9550</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1239</v>
+      </c>
+      <c r="C13" t="n">
+        <v>63</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>07-07-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>9566</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Hungary</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Hungaroring</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>21-07-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>9574</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Belgium</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Spa-Francorchamps</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>28-07-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>9582</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Netherlands</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Zandvoort</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>25-08-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>9590</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Monza</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>01-09-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>9598</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Azerbaijan</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Baku</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>15-09-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>9606</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Singapore</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Singapore</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>22-09-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>9617</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Austin</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>20-10-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>9625</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Mexico</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Mexico City</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>27-10-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>9636</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Brazil</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Interlagos</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>03-11-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>9644</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>United States</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Las Vegas</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>24-11-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>9655</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Qatar</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Lusail</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>01-12-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>9662</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>United Arab Emirates</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Yas Marina Circuit</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>08-12-2024</t>
-        </is>
+          <t>30-06-2024</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>